<commit_message>
fixed misc data import bugs
</commit_message>
<xml_diff>
--- a/raw_data/English_WG/EnglishWG_Byers.xlsx
+++ b/raw_data/English_WG/EnglishWG_Byers.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12520" windowHeight="14100"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12520" windowHeight="14100" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8622" uniqueCount="750">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8624" uniqueCount="750">
   <si>
     <t>A1Eng</t>
   </si>
@@ -2798,8 +2798,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="85">
+  <cellStyleXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2945,7 +2947,7 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="85">
+  <cellStyles count="87">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2988,6 +2990,7 @@
     <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -3030,6 +3033,7 @@
     <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3329,7 +3333,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:RE42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BJ1" workbookViewId="0">
+    <sheetView topLeftCell="BJ1" workbookViewId="0">
       <selection activeCell="BM2" sqref="BM2"/>
     </sheetView>
   </sheetViews>
@@ -43853,10 +43857,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -43962,24 +43966,20 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="11" t="s">
-        <v>593</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>594</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>594</v>
-      </c>
+        <v>592</v>
+      </c>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="11" t="s">
         <v>593</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>577</v>
+        <v>594</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>577</v>
+        <v>594</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -43987,21 +43987,21 @@
         <v>593</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="11" t="s">
-        <v>574</v>
+        <v>593</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>575</v>
+        <v>578</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -44009,70 +44009,88 @@
         <v>574</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="11" t="s">
-        <v>595</v>
+        <v>574</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>576</v>
+        <v>579</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>594</v>
+        <v>579</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="11" t="s">
-        <v>595</v>
-      </c>
-      <c r="B17" s="11" t="s">
-        <v>577</v>
-      </c>
-      <c r="C17" s="11" t="s">
-        <v>577</v>
-      </c>
+        <v>574</v>
+      </c>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="11" t="s">
         <v>595</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>578</v>
+        <v>594</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="11" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>449</v>
+        <v>577</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>449</v>
+        <v>577</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="11" t="s">
+        <v>595</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>578</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="11" t="s">
         <v>596</v>
       </c>
-      <c r="B20" s="11" t="s">
+      <c r="B21" s="11" t="s">
+        <v>449</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="11" t="s">
+        <v>596</v>
+      </c>
+      <c r="B22" s="11" t="s">
         <v>382</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="C22" s="11" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="8"/>
-      <c r="B21" s="8"/>
+    <row r="23" spans="1:3">
+      <c r="A23" s="8"/>
+      <c r="B23" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
renamed field/value mapping sheets for excel/csv consistency
</commit_message>
<xml_diff>
--- a/raw_data/English_WG/EnglishWG_Byers.xlsx
+++ b/raw_data/English_WG/EnglishWG_Byers.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14100" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14100" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
-    <sheet name="field_mapping" sheetId="4" r:id="rId2"/>
-    <sheet name="value_mapping" sheetId="5" r:id="rId3"/>
+    <sheet name="fields" sheetId="4" r:id="rId2"/>
+    <sheet name="values" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -38365,7 +38365,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E526"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B501" sqref="B501"/>
     </sheetView>
   </sheetViews>
@@ -46891,7 +46891,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>

</xml_diff>